<commit_message>
Added DataTable loading functionality and ActionMaker GameMode
</commit_message>
<xml_diff>
--- a/Content/Sample/Excel/Sample1.xlsx
+++ b/Content/Sample/Excel/Sample1.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unreal Projects\excel_plugin\Plugins\ExcelImporter\Content\Sample\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Unreal Projects\ShowSystemSample\Plugins\ExcelImporter\Content\Sample\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0AAC10-D4A4-425F-8352-0AF8A2FD232F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD7365-A09C-42FF-A1F6-2C12499B8829}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6495" yWindow="2565" windowWidth="21600" windowHeight="11835" xr2:uid="{CC7A5549-E528-4DF5-A60D-2C2DFAB64B64}"/>
+    <workbookView xWindow="-26010" yWindow="3435" windowWidth="21600" windowHeight="11835" xr2:uid="{CC7A5549-E528-4DF5-A60D-2C2DFAB64B64}"/>
   </bookViews>
   <sheets>
-    <sheet name="Skill" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>